<commit_message>
new flet version config
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,17 +493,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nome Procedimento</t>
+          <t>Descrição do Procedimento</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Quantidade</t>
+          <t>Quantidade do Procedimento</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Valor Total Procedimento</t>
+          <t>Valor do Procedimento</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -530,22 +530,22 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>DOSAGEM DE CALCIO</t>
+          <t>ACOMPANHAMENTO DE PACIENTES NO PRÉ TRANSPLANTE DE RIM</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>R$ 2,78</t>
+          <t>R$ 324,00</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>BÁSICO</t>
+          <t>CONSULTA</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -555,331 +555,35 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>R$ 25,00</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>R$ 0,83</t>
+          <t>R$ 25,00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>DOSAGEM DE FOSFORO</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>R$ 2,78</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="n"/>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n"/>
+      <c r="E3" s="3" t="n"/>
+      <c r="F3" s="4" t="n"/>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>R$ 0,83</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>DOSAGEM DE POTASSIO</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>R$ 2,78</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>R$ 0,83</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>DOSAGEM DE SODIO</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>R$ 2,78</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>R$ 0,83</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>DOSAGEM DE TRANSAMINASE GLUTAMICO-PIRUVICA (TGP)</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>R$ 3,02</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>R$ 0,91</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>DOSAGEM DE UREIA</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>R$ 5,55</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>R$ 1,66</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>DOSAGEM DE HEMOGLOBINA</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>R$ 2,30</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>R$ 0,69</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>HEMATOCRITO</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>R$ 2,30</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>BÁSICO</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>SIM</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>30%</t>
-        </is>
-      </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>R$ 0,69</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>HEMODIÁLISE (MÁXIMO 3 SESSÕES POR SEMANA)</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>10.0</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>R$ 3.614,55</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>AMBULATORIAL</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>NÃO</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="4" t="n"/>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>R$ 7,29</t>
+          <t>R$ 25,00</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Lista da pagina renomear atualiza agora ao adicionar outra lista
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,7 +540,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>R$ 34,50</t>
+          <t>R$ 69,00</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -560,14 +560,14 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>R$ 10,35</t>
+          <t>R$ 20,70</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>AUDIOMETRIA TONAL LIMIAR (VIA AEREA / OSSEA)</t>
+          <t>LOGOAUDIOMETRIA (LDV-IRF-LRF)</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>R$ 31,50</t>
+          <t>R$ 78,75</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -597,14 +597,14 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>R$ 9,45</t>
+          <t>R$ 23,62</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>LOGOAUDIOMETRIA (LDV-IRF-LRF)</t>
+          <t>AUDIOMETRIA EM CAMPO LIVRE</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -614,7 +614,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>R$ 39,38</t>
+          <t>R$ 60,39</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -634,14 +634,14 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>R$ 11,81</t>
+          <t>R$ 18,12</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>AVALIACAO P/ DIAGNOSTICO DIFERENCIAL DE DEFICIENCIA AUDITIVA</t>
+          <t>AUDIOMETRIA TONAL LIMIAR (VIA AEREA / OSSEA)</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -651,50 +651,87 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>R$ 69,84</t>
+          <t>R$ 63,00</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>CONSULTA</t>
+          <t>BÁSICO</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>NÃO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>30%</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>R$ 18,90</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>ACOMPANHAMENTO DE PACIENTE P/ ADAPTACAO DE APARELHO DE AMPLIFICACAO SONORA INDIVIDUAL (AASI) UNI / BILATERAL</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>R$ 32,52</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>CONSULTA</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>SIM</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>30%</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>R$ 9,76</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="4" t="n"/>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>R$ 31,61</t>
+      <c r="B7" s="3" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
+      <c r="F7" s="4" t="n"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>R$ 91,10</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>